<commit_message>
Reszied Participant Bar Charts
</commit_message>
<xml_diff>
--- a/Documents/Script_Documents/Visuals/SNW/Results Formatting for Final Paper.xlsx
+++ b/Documents/Script_Documents/Visuals/SNW/Results Formatting for Final Paper.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17739\Desktop\ST 542 Statistical Practice\FinalProject\FACES\Documents\Script_Documents\Visuals\SNW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAF4EAB-9C82-4C8B-915F-5D1A58858A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6703211A-9E5B-416C-80F1-579AC87F6A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FD14D3D4-2E69-4195-8680-CA3F37A8090A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{FD14D3D4-2E69-4195-8680-CA3F37A8090A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Table 1: Results from Wilcoxon Signed-Rank Test</t>
   </si>
@@ -47,6 +48,24 @@
   <si>
     <t>Table 4: Results from Wilcoxon Signed-Rank Test</t>
   </si>
+  <si>
+    <t>Figure 2: Bar chart for FES Total Scores</t>
+  </si>
+  <si>
+    <t>Figure 3: Bar chart for AKS Total Scores</t>
+  </si>
+  <si>
+    <t>Figure 4: Bar chart for FACES Total Scores</t>
+  </si>
+  <si>
+    <t>Figure 5: Bar chart for FPPS Total Scores</t>
+  </si>
+  <si>
+    <t>Figure 6: Bar chart for SCS Total Scores</t>
+  </si>
+  <si>
+    <t>Figure 7: Bar chart for SEAS Total Scores</t>
+  </si>
 </sst>
 </file>
 
@@ -57,7 +76,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +100,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -113,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -125,6 +151,8 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -313,6 +341,275 @@
         <a:xfrm>
           <a:off x="571500" y="4486275"/>
           <a:ext cx="3295238" cy="1276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{727725A7-C6F2-4A4F-A3C8-F6C31D875DE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="657226" y="1143000"/>
+          <a:ext cx="6000750" cy="4000499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>64009</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>23620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{297847DB-7F62-4CB0-AEFB-FC5980DDA65A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="1352548"/>
+          <a:ext cx="6007609" cy="4005072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>104777</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6044A9B9-3A51-47B1-9673-3B2787AD9AF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12906377" y="1155702"/>
+          <a:ext cx="5953123" cy="3968749"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>436007</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>17620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CD8102-1481-4E43-97E6-DB4DD1C2F1C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="6057899"/>
+          <a:ext cx="5798582" cy="3865721"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9523</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C27D5C-34BA-4B05-88C5-8E83510AB63B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6715123" y="6057899"/>
+          <a:ext cx="5686427" cy="3790951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>44448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE277FEB-168F-417A-BA34-0BDC6A2F5858}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="10820399"/>
+          <a:ext cx="5553075" cy="3702049"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -623,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A881E4A-1B16-46A3-8C97-5736DA65DFA6}">
   <dimension ref="A4:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,4 +1383,49 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40086675-5D05-4F53-9923-2E00FBB0E4BA}">
+  <dimension ref="C28:W77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P68" sqref="P68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="W28" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="M29" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C53" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M53" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formatting tables and figures for final report.
</commit_message>
<xml_diff>
--- a/Documents/Script_Documents/Visuals/SNW/Results Formatting for Final Paper.xlsx
+++ b/Documents/Script_Documents/Visuals/SNW/Results Formatting for Final Paper.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17739\Desktop\ST 542 Statistical Practice\FinalProject\FACES\Documents\Script_Documents\Visuals\SNW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6703211A-9E5B-416C-80F1-579AC87F6A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1535112E-0182-4F4A-8866-BE84ED77CCF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{FD14D3D4-2E69-4195-8680-CA3F37A8090A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{FD14D3D4-2E69-4195-8680-CA3F37A8090A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t>Table 1: Results from Wilcoxon Signed-Rank Test</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>W = Test Statistic from Wilcoxon Test, p = p-value, ES = Effect Size</t>
   </si>
@@ -49,22 +47,43 @@
     <t>Table 4: Results from Wilcoxon Signed-Rank Test</t>
   </si>
   <si>
-    <t>Figure 2: Bar chart for FES Total Scores</t>
+    <t>Table 1: Missing Data</t>
   </si>
   <si>
-    <t>Figure 3: Bar chart for AKS Total Scores</t>
+    <t>Table 5: Results from Wilcoxon Signed-Rank Test</t>
   </si>
   <si>
-    <t>Figure 4: Bar chart for FACES Total Scores</t>
+    <t>Figure 1: Bar chart for FES Total Scores</t>
   </si>
   <si>
-    <t>Figure 5: Bar chart for FPPS Total Scores</t>
+    <t>Figure 2: Bar chart for AKS Total Scores</t>
   </si>
   <si>
-    <t>Figure 6: Bar chart for SCS Total Scores</t>
+    <t>Figure 3: Bar chart for FACES Total Scores</t>
   </si>
   <si>
-    <t>Figure 7: Bar chart for SEAS Total Scores</t>
+    <t>Figure 4: Bar chart for FPPS Total Scores</t>
+  </si>
+  <si>
+    <t>Figure 5: Bar chart for SCS Total Scores</t>
+  </si>
+  <si>
+    <t>Figure 6: Bar chart for SEAS Total Scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 7: A Boxplot for each survey. </t>
+  </si>
+  <si>
+    <t>Figure 8: Q-Q (Quantile-Quantile) Plot for Standardized Differences between Pre and Post Scores</t>
+  </si>
+  <si>
+    <t>Participant # 5</t>
+  </si>
+  <si>
+    <t>Figure 9: Plot of Power by Sample Size.</t>
+  </si>
+  <si>
+    <t>Figure 10: Plot of Power by Sample Size.</t>
   </si>
 </sst>
 </file>
@@ -76,7 +95,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +130,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -139,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -153,6 +180,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -341,6 +372,50 @@
         <a:xfrm>
           <a:off x="571500" y="4486275"/>
           <a:ext cx="3295238" cy="1276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>8831</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>56723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E3272B8-FF10-477E-83C4-562EE1B4E135}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12744450" y="1209675"/>
+          <a:ext cx="5552381" cy="3419048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -614,6 +689,363 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>549010</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E10021C-D6E7-44F9-8F50-4CE4967527FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1590674" y="942974"/>
+          <a:ext cx="8094716" cy="4562476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>570667</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>113786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B79F925-502C-45B6-9148-F448B0FF75D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="6286500"/>
+          <a:ext cx="6666667" cy="4114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78771567-6BFC-466C-9766-04D394832360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8067675" y="6257925"/>
+          <a:ext cx="628650" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>554356</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>97156</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FBA787D-A8AB-4826-A23F-A15A0541257F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8726806" y="6431281"/>
+          <a:ext cx="369569" cy="283844"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>514741</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B91CB508-5269-4F44-9ED2-C90AE09D158E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12372975" y="981075"/>
+          <a:ext cx="5105791" cy="3114675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>45774</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C21CEC38-38F5-4FF2-BE8D-ED583259D1E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12125325" y="5495925"/>
+          <a:ext cx="5520744" cy="3348990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -918,19 +1350,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A881E4A-1B16-46A3-8C97-5736DA65DFA6}">
-  <dimension ref="A4:S32"/>
+  <dimension ref="A4:AD32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:19" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -949,8 +1428,18 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U8" s="1"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -969,8 +1458,18 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -989,8 +1488,18 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1009,8 +1518,18 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="4"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1029,8 +1548,18 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1049,8 +1578,18 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="4"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1069,8 +1608,18 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1087,11 +1636,21 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="4"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1111,11 +1670,21 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="4"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1126,7 +1695,7 @@
       <c r="I17" s="4"/>
       <c r="K17" s="1"/>
       <c r="L17" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1135,8 +1704,18 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="4"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1153,8 +1732,54 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="1"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1173,8 +1798,18 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1193,8 +1828,18 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1213,8 +1858,20 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U24" s="1"/>
+      <c r="V24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1233,8 +1890,18 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="4"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1253,8 +1920,18 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
       <c r="S26" s="4"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1273,8 +1950,18 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="4"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1294,7 +1981,7 @@
       <c r="R28" s="6"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1312,7 +1999,7 @@
       <c r="R29" s="6"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="7" t="s">
         <v>3</v>
@@ -1326,7 +2013,7 @@
       <c r="I30" s="4"/>
       <c r="K30" s="1"/>
       <c r="L30" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1336,10 +2023,10 @@
       <c r="R30" s="6"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1350,7 +2037,7 @@
       <c r="I31" s="4"/>
       <c r="K31" s="1"/>
       <c r="L31" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1360,7 +2047,7 @@
       <c r="R31" s="6"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1389,43 +2076,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40086675-5D05-4F53-9923-2E00FBB0E4BA}">
   <dimension ref="C28:W77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P68" sqref="P68"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C28" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W28" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="M29" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="M29" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C53" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCCA3CD-DE33-4B05-AAF8-50400BE8A0CA}">
+  <dimension ref="C5:U56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.109375" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="D6"/>
+      <c r="U6"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="U24" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D30" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="U32"/>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O38" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="U50" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D56" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created Summary Stat tables for Median and IQR
</commit_message>
<xml_diff>
--- a/Documents/Script_Documents/Visuals/SNW/Results Formatting for Final Paper.xlsx
+++ b/Documents/Script_Documents/Visuals/SNW/Results Formatting for Final Paper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17739\Desktop\ST 542 Statistical Practice\FinalProject\FACES\Documents\Script_Documents\Visuals\SNW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1535112E-0182-4F4A-8866-BE84ED77CCF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39F3F38-61BF-40BF-8D4D-576B0D469342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{FD14D3D4-2E69-4195-8680-CA3F37A8090A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FD14D3D4-2E69-4195-8680-CA3F37A8090A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>W = Test Statistic from Wilcoxon Test, p = p-value, ES = Effect Size</t>
   </si>
@@ -85,6 +85,12 @@
   <si>
     <t>Figure 10: Plot of Power by Sample Size.</t>
   </si>
+  <si>
+    <t>Table 2: Median by Survey for Pre Experimental, Pre Control, Post Experimental, and Post Control Groups</t>
+  </si>
+  <si>
+    <t>Table 3: Interquartile Range (IQR) by Survey for Pre Experimental, Pre Control, Post Experimental, and Post Control Groups</t>
+  </si>
 </sst>
 </file>
 
@@ -95,7 +101,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +144,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -166,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -184,6 +197,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -416,6 +430,94 @@
         <a:xfrm>
           <a:off x="12744450" y="1209675"/>
           <a:ext cx="5552381" cy="3419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>151277</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9249</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0121440A-50DA-4771-BB62-1AB95DC1790D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="314325" y="7705725"/>
+          <a:ext cx="8980952" cy="2209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>132251</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>180710</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB18D2B1-9C66-4447-8E43-0052F6A54C76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10848975" y="7772400"/>
+          <a:ext cx="8790476" cy="2123810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1350,18 +1452,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A881E4A-1B16-46A3-8C97-5736DA65DFA6}">
-  <dimension ref="A4:AD32"/>
+  <dimension ref="A4:AD56"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:30" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
@@ -1373,7 +1475,7 @@
       <c r="AC4" s="11"/>
       <c r="AD4" s="11"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1385,7 +1487,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1397,7 +1499,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1409,7 +1511,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1439,7 +1541,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1469,7 +1571,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1499,7 +1601,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1529,7 +1631,7 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1559,7 +1661,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1589,7 +1691,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1619,7 +1721,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1647,7 +1749,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="7" t="s">
         <v>1</v>
@@ -1681,7 +1783,7 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="8" t="s">
         <v>0</v>
@@ -1715,7 +1817,7 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1743,7 +1845,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
@@ -1755,7 +1857,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
@@ -1767,7 +1869,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -1779,7 +1881,7 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1809,7 +1911,7 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1839,7 +1941,7 @@
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1871,7 +1973,7 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1901,7 +2003,7 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1931,7 +2033,7 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1961,7 +2063,7 @@
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1981,7 +2083,7 @@
       <c r="R28" s="6"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1999,7 +2101,7 @@
       <c r="R29" s="6"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="7" t="s">
         <v>3</v>
@@ -2023,7 +2125,7 @@
       <c r="R30" s="6"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="8" t="s">
         <v>0</v>
@@ -2047,7 +2149,7 @@
       <c r="R31" s="6"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2065,6 +2167,37 @@
       <c r="R32" s="6"/>
       <c r="S32" s="1"/>
     </row>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="S52" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2076,16 +2209,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40086675-5D05-4F53-9923-2E00FBB0E4BA}">
   <dimension ref="C28:W77"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="9"/>
+    <col min="1" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="28" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C28" s="10" t="s">
         <v>6</v>
       </c>
@@ -2093,12 +2226,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
       <c r="M29" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C53" s="10" t="s">
         <v>9</v>
       </c>
@@ -2106,7 +2239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="10" t="s">
         <v>11</v>
       </c>
@@ -2121,46 +2254,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCCA3CD-DE33-4B05-AAF8-50400BE8A0CA}">
   <dimension ref="C5:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="9"/>
+    <col min="1" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C5"/>
     </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D6"/>
       <c r="U6"/>
     </row>
-    <row r="24" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="U24" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
       <c r="U32"/>
     </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O38" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:21" x14ac:dyDescent="0.25">
       <c r="U50" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D56" s="10" t="s">
         <v>13</v>
       </c>

</xml_diff>